<commit_message>
Fixed some test errors
</commit_message>
<xml_diff>
--- a/ERP.xlsx
+++ b/ERP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -158,25 +158,22 @@
     <t xml:space="preserve">Question: Which items are sold between two given dates? (from_date &lt; sale_date &lt; to_date) Returns list of lists</t>
   </si>
   <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_counts_by_manufacturers(table)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question: How many different kinds of game are available of each manufacturer?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_average_by_manufacturer(table, manufacturer):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question: What is the average amount of games in stock of a given manufacturer?</t>
+  </si>
+  <si>
     <t xml:space="preserve">In progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_counts_by_manufacturers(table)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question: How many different kinds of game are available of each manufacturer?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">get_average_by_manufacturer(table, manufacturer):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question: What is the average amount of games in stock of a given manufacturer?</t>
   </si>
   <si>
     <t xml:space="preserve">ui</t>
@@ -232,12 +229,13 @@
     <numFmt numFmtId="167" formatCode="YYYY\.MM\.DD"/>
     <numFmt numFmtId="168" formatCode="YYYY\.M\.D\."/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -256,87 +254,11 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF2C3E50"/>
       <name val="&quot;Source Sans Pro&quot;"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -344,6 +266,7 @@
       <color rgb="FF2C3E50"/>
       <name val="&quot;Source Sans Pro&quot;"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -351,66 +274,27 @@
       <color rgb="FF2C3E50"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFFCE5CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD9EAD3"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -421,7 +305,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
     <fill>
@@ -433,13 +317,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFCE5CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFF450"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -451,7 +335,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC9DAF8"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
@@ -461,27 +345,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -548,7 +417,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -572,345 +441,278 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="16" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="16" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="16" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
       <font>
         <name val="Arial"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -924,45 +726,45 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFEFEFEF"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFD9EAD3"/>
+      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFC9DAF8"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFF450"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFEFEFEF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFD9EAD3"/>
+      <rgbColor rgb="FFFFF450"/>
       <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFCE5CD"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -977,8 +779,8 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF2C3E50"/>
-      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -992,7 +794,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1615,7 +1417,7 @@
         <v>36</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="H16" s="26"/>
       <c r="I16" s="27"/>
@@ -1642,20 +1444,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="D17" s="30" t="s">
         <v>47</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>48</v>
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="28" t="s">
         <v>30</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H17" s="43"/>
       <c r="I17" s="33"/>
@@ -1723,17 +1525,17 @@
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" s="28"/>
       <c r="F19" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>49</v>
+        <v>24</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="H19" s="34"/>
       <c r="I19" s="33"/>
@@ -1760,13 +1562,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="D20" s="47" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>54</v>
       </c>
       <c r="E20" s="45"/>
       <c r="F20" s="45" t="s">
@@ -1803,10 +1605,10 @@
       </c>
       <c r="B21" s="52"/>
       <c r="C21" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="54" t="s">
         <v>55</v>
-      </c>
-      <c r="D21" s="54" t="s">
-        <v>56</v>
       </c>
       <c r="E21" s="52"/>
       <c r="F21" s="52" t="s">
@@ -1843,10 +1645,10 @@
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="54" t="s">
         <v>57</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>58</v>
       </c>
       <c r="E22" s="52"/>
       <c r="F22" s="52" t="s">
@@ -1883,10 +1685,10 @@
       </c>
       <c r="B23" s="52"/>
       <c r="C23" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="54" t="s">
         <v>59</v>
-      </c>
-      <c r="D23" s="54" t="s">
-        <v>60</v>
       </c>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
@@ -1923,10 +1725,10 @@
       </c>
       <c r="B24" s="52"/>
       <c r="C24" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="54" t="s">
         <v>61</v>
-      </c>
-      <c r="D24" s="54" t="s">
-        <v>62</v>
       </c>
       <c r="E24" s="52"/>
       <c r="F24" s="52" t="s">
@@ -1962,13 +1764,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="D25" s="61" t="s">
         <v>64</v>
-      </c>
-      <c r="D25" s="61" t="s">
-        <v>65</v>
       </c>
       <c r="E25" s="59"/>
       <c r="F25" s="59" t="s">

</xml_diff>